<commit_message>
libros de programas procesados
</commit_message>
<xml_diff>
--- a/data/procesados/cp_bibliografia_programas.xlsx
+++ b/data/procesados/cp_bibliografia_programas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Practica-Biblioteca\data\procesados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EA7095-71C0-49CA-80F5-4DF195BC86BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D78361-E111-4561-9A16-20B2F6F9113A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="82">
   <si>
     <t>Carrera</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Cálculo en una Variable $ James Stewart</t>
   </si>
   <si>
-    <t>STEWART, James $ Cálculo de una variable- Trascendentes y tempranas</t>
-  </si>
-  <si>
-    <t>STEWART, James $ Precálculo - Matemáticas para el cálculo</t>
-  </si>
-  <si>
     <t>El tutorial de Python. $ Python Software Foundation.</t>
   </si>
   <si>
@@ -269,6 +263,9 @@
   </si>
   <si>
     <t>Probabilidad y estadística: enfoque por competencias. $ GUTIERREZ BANEGAS, A. L.</t>
+  </si>
+  <si>
+    <t>Cálculo de una variable- Trascendentes y tempranas $ STEWART, James</t>
   </si>
 </sst>
 </file>
@@ -642,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B86" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -727,7 +724,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -782,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,7 +790,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,7 +812,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,7 +845,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +867,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,7 +878,7 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,7 +889,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,7 +900,7 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +911,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,7 +922,7 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,7 +933,7 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +944,7 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +955,7 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,7 +1010,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1021,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,7 +1032,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1054,7 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1068,7 +1065,7 @@
         <v>19</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,7 +1076,7 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,7 +1087,7 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,7 +1098,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,7 +1109,7 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,7 +1120,7 @@
         <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,7 +1142,7 @@
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,7 +1164,7 @@
         <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1189,7 +1186,7 @@
         <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1200,7 +1197,7 @@
         <v>21</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1211,7 +1208,7 @@
         <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1222,7 +1219,7 @@
         <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1233,7 +1230,7 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1244,7 +1241,7 @@
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,7 +1252,7 @@
         <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1266,7 +1263,7 @@
         <v>23</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1277,7 +1274,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1288,7 +1285,7 @@
         <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,7 +1296,7 @@
         <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,7 +1307,7 @@
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1321,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1332,7 +1329,7 @@
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1343,7 +1340,7 @@
         <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1354,7 +1351,7 @@
         <v>24</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1365,7 +1362,7 @@
         <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1373,7 @@
         <v>24</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,7 +1384,7 @@
         <v>24</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,7 +1395,7 @@
         <v>24</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,7 +1406,7 @@
         <v>24</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1417,7 @@
         <v>24</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,7 +1428,7 @@
         <v>24</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1442,7 +1439,7 @@
         <v>24</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1450,7 @@
         <v>24</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,7 +1461,7 @@
         <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,7 +1472,7 @@
         <v>25</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1483,7 @@
         <v>26</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,7 +1516,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1530,7 +1527,7 @@
         <v>28</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1541,7 +1538,7 @@
         <v>28</v>
       </c>
       <c r="C81" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,7 +1549,7 @@
         <v>28</v>
       </c>
       <c r="C82" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,7 +1560,7 @@
         <v>28</v>
       </c>
       <c r="C83" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,7 +1571,7 @@
         <v>28</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1585,7 +1582,7 @@
         <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,7 +1593,7 @@
         <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,7 +1604,7 @@
         <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1618,7 +1615,7 @@
         <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1629,7 +1626,7 @@
         <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1640,7 +1637,7 @@
         <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,7 +1648,7 @@
         <v>29</v>
       </c>
       <c r="C91" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1662,7 +1659,7 @@
         <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1673,7 +1670,7 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1681,7 @@
         <v>29</v>
       </c>
       <c r="C94" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,7 +1692,7 @@
         <v>30</v>
       </c>
       <c r="C95" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,7 +1703,7 @@
         <v>30</v>
       </c>
       <c r="C96" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,7 +1714,7 @@
         <v>30</v>
       </c>
       <c r="C97" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>